<commit_message>
Pushing changes to P2P Data Input.xlsx
</commit_message>
<xml_diff>
--- a/P2P Data Input.xlsx
+++ b/P2P Data Input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Matlab Folder\Project NTNU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Master's\NTNU\PCDG_Github\PCDGModel-LocalCommunities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D366B8DB-09A9-4B96-870D-B50A2FA59047}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9F9E94-DF8D-4A10-8C88-DC62806F08DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8435,7 +8435,7 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="E47" sqref="E47:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Few sentences added in the welcome tab
</commit_message>
<xml_diff>
--- a/P2P Data Input.xlsx
+++ b/P2P Data Input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Master's\NTNU\PCDG_Github\PCDGModel-LocalCommunities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932ACA2C-C4A6-4209-96E8-3D48D4834E33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41ADE45-B5DB-47CE-B0E4-F2FEA523390E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome" sheetId="7" r:id="rId1"/>
@@ -192,13 +192,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:rowOff>182878</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>68579</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -213,8 +213,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="219075" y="190499"/>
-          <a:ext cx="4305299" cy="2657476"/>
+          <a:off x="219075" y="182878"/>
+          <a:ext cx="4305299" cy="3360421"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -248,9 +248,86 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Welcome!</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IN">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>- The Excel spreadsheet is split into six different sheets: Sets, Demand_houses, Elec_price, Wind_Input, PV_input, and Battery_input. </a:t>
+            <a:t>- The Excel spreadsheet is split into six different sheets: </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>   Demand, Electricity</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> P</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>rice, Wind Data, PV</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Data and Grid Tariff</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Demand</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>represents the power demand per time period. </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -259,7 +336,23 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>- Demand_houses represents the power demand per time period. </a:t>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Electricity</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> P</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>rice </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>represents the electricity price per time period.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -268,7 +361,35 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>- Elec_price represents the electricity price per time period.</a:t>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Wind</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> Data </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>PV</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> Data </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>represent the wind and PV per time period, for all houses that have solar and wind turbine systems.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -277,7 +398,19 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>- Wind_input and PV_input represent the wind and PV per time period, for all houses that have solar and wind turbine systems.</a:t>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Grid Tariff </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>represents the feed-in</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>- tariff for each time step</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -286,17 +419,25 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>- Battery_input represents the various characteristics of home batteries. Currently our model is set up assuming everyone within the trading network has the same battery. </a:t>
+            <a:t>Currently our model is set up assuming everyone within the trading network has the same battery.  A common battery can</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> be allocated to all participating houses.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>We have also built in a case where none of the houses posess a battery.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Welcome!</a:t>
-          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -570,7 +711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E8A0DD-D966-47A7-ABCA-5164E3F7264C}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -6061,7 +6202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="AF9" sqref="AF9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Renamed dataset25housesninemonths.xlsx to 9 Month UK Dataset for 25 houses
</commit_message>
<xml_diff>
--- a/P2P Data Input.xlsx
+++ b/P2P Data Input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Master's\NTNU\PCDG_Github\PCDGModel-LocalCommunities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41ADE45-B5DB-47CE-B0E4-F2FEA523390E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D039185-805C-4D76-85F2-67443DD8144B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome" sheetId="7" r:id="rId1"/>
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E8A0DD-D966-47A7-ABCA-5164E3F7264C}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -802,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z49"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AB12" sqref="AB12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>